<commit_message>
test: improve dummy log
</commit_message>
<xml_diff>
--- a/cmd/ayd/testdata/log.xlsx
+++ b/cmd/ayd/testdata/log.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
-    <t>time (JST)</t>
+    <t>time (UTC)</t>
   </si>
   <si>
     <t>status</t>
@@ -567,7 +567,7 @@
     </row>
     <row r="2" s="1" customFormat="true">
       <c r="A2" s="2">
-        <v>44199.00283564815</v>
+        <v>44198.62783564815</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -584,7 +584,7 @@
     </row>
     <row r="3" s="5" customFormat="true">
       <c r="A3" s="6">
-        <v>44199.00283564815</v>
+        <v>44198.62783564815</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>8</v>
@@ -601,7 +601,7 @@
     </row>
     <row r="4" s="1" customFormat="true">
       <c r="A4" s="2">
-        <v>44199.002847222226</v>
+        <v>44198.627847222226</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
@@ -618,7 +618,7 @@
     </row>
     <row r="5" s="1" customFormat="true">
       <c r="A5" s="2">
-        <v>44199.002847222226</v>
+        <v>44198.627847222226</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
@@ -632,10 +632,13 @@
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="F5" s="1">
+        <v>1.234</v>
+      </c>
     </row>
     <row r="6" s="1" customFormat="true">
       <c r="A6" s="2">
-        <v>44199.002858796295</v>
+        <v>44198.627858796295</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
@@ -652,7 +655,7 @@
     </row>
     <row r="7" s="9" customFormat="true">
       <c r="A7" s="10">
-        <v>44199.00287037037</v>
+        <v>44198.62787037037</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>14</v>
@@ -672,7 +675,7 @@
     </row>
     <row r="8" s="13" customFormat="true">
       <c r="A8" s="14">
-        <v>44199.00288194444</v>
+        <v>44198.62788194444</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>17</v>
@@ -695,7 +698,7 @@
     </row>
     <row r="9" s="1" customFormat="true">
       <c r="A9" s="2">
-        <v>44200.00283564815</v>
+        <v>44199.62783564815</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
chore: follow breaking change of excelize
</commit_message>
<xml_diff>
--- a/cmd/ayd/testdata/log.xlsx
+++ b/cmd/ayd/testdata/log.xlsx
@@ -268,120 +268,120 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
+<theme xmlns="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <themeElements>
+    <clrScheme name="Office">
+      <dk1>
+        <sysClr val="windowText" lastClr="000000"/>
+      </dk1>
+      <lt1>
+        <sysClr val="window" lastClr="FFFFFF"/>
+      </lt1>
+      <dk2>
+        <srgbClr val="44546A"/>
+      </dk2>
+      <lt2>
+        <srgbClr val="E7E6E6"/>
+      </lt2>
+      <accent1>
+        <srgbClr val="5B9BD5"/>
+      </accent1>
+      <accent2>
+        <srgbClr val="ED7D31"/>
+      </accent2>
+      <accent3>
+        <srgbClr val="A5A5A5"/>
+      </accent3>
+      <accent4>
+        <srgbClr val="FFC000"/>
+      </accent4>
+      <accent5>
+        <srgbClr val="4472C4"/>
+      </accent5>
+      <accent6>
+        <srgbClr val="70AD47"/>
+      </accent6>
+      <hlink>
+        <srgbClr val="0563C1"/>
+      </hlink>
+      <folHlink>
+        <srgbClr val="954F72"/>
+      </folHlink>
+    </clrScheme>
+    <fontScheme name="Office">
+      <majorFont>
+        <latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <ea typeface=""/>
+        <cs typeface=""/>
+        <font script="Jpan" typeface="游ゴシック Light"/>
+        <font script="Hang" typeface="맑은 고딕"/>
+        <font script="Hans" typeface="等线 Light"/>
+        <font script="Hant" typeface="新細明體"/>
+        <font script="Arab" typeface="Times New Roman"/>
+        <font script="Hebr" typeface="Times New Roman"/>
+        <font script="Thai" typeface="Tahoma"/>
+        <font script="Ethi" typeface="Nyala"/>
+        <font script="Beng" typeface="Vrinda"/>
+        <font script="Gujr" typeface="Shruti"/>
+        <font script="Khmr" typeface="MoolBoran"/>
+        <font script="Knda" typeface="Tunga"/>
+        <font script="Guru" typeface="Raavi"/>
+        <font script="Cans" typeface="Euphemia"/>
+        <font script="Cher" typeface="Plantagenet Cherokee"/>
+        <font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <font script="Tibt" typeface="Microsoft Himalaya"/>
+        <font script="Thaa" typeface="MV Boli"/>
+        <font script="Deva" typeface="Mangal"/>
+        <font script="Telu" typeface="Gautami"/>
+        <font script="Taml" typeface="Latha"/>
+        <font script="Syrc" typeface="Estrangelo Edessa"/>
+        <font script="Orya" typeface="Kalinga"/>
+        <font script="Mlym" typeface="Kartika"/>
+        <font script="Laoo" typeface="DokChampa"/>
+        <font script="Sinh" typeface="Iskoola Pota"/>
+        <font script="Mong" typeface="Mongolian Baiti"/>
+        <font script="Viet" typeface="Times New Roman"/>
+        <font script="Uigh" typeface="Microsoft Uighur"/>
+        <font script="Geor" typeface="Sylfaen"/>
+      </majorFont>
+      <minorFont>
+        <latin typeface="Calibri" panose="020F0502020204030204"/>
+        <ea typeface=""/>
+        <cs typeface=""/>
+        <font script="Jpan" typeface="游ゴシック"/>
+        <font script="Hang" typeface="맑은 고딕"/>
+        <font script="Hans" typeface="等线"/>
+        <font script="Hant" typeface="新細明體"/>
+        <font script="Arab" typeface="Arial"/>
+        <font script="Hebr" typeface="Arial"/>
+        <font script="Thai" typeface="Tahoma"/>
+        <font script="Ethi" typeface="Nyala"/>
+        <font script="Beng" typeface="Vrinda"/>
+        <font script="Gujr" typeface="Shruti"/>
+        <font script="Khmr" typeface="DaunPenh"/>
+        <font script="Knda" typeface="Tunga"/>
+        <font script="Guru" typeface="Raavi"/>
+        <font script="Cans" typeface="Euphemia"/>
+        <font script="Cher" typeface="Plantagenet Cherokee"/>
+        <font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <font script="Tibt" typeface="Microsoft Himalaya"/>
+        <font script="Thaa" typeface="MV Boli"/>
+        <font script="Deva" typeface="Mangal"/>
+        <font script="Telu" typeface="Gautami"/>
+        <font script="Taml" typeface="Latha"/>
+        <font script="Syrc" typeface="Estrangelo Edessa"/>
+        <font script="Orya" typeface="Kalinga"/>
+        <font script="Mlym" typeface="Kartika"/>
+        <font script="Laoo" typeface="DokChampa"/>
+        <font script="Sinh" typeface="Iskoola Pota"/>
+        <font script="Mong" typeface="Mongolian Baiti"/>
+        <font script="Viet" typeface="Arial"/>
+        <font script="Uigh" typeface="Microsoft Uighur"/>
+        <font script="Geor" typeface="Sylfaen"/>
+      </minorFont>
+    </fontScheme>
+    <fmtScheme name="Office">
+      <fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -437,8 +437,8 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
+      </fillStyleLst>
+      <lnStyleLst>
         <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -460,8 +460,8 @@
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
+      </lnStyleLst>
+      <effectStyleLst>
         <a:effectStyle>
           <a:effectLst/>
         </a:effectStyle>
@@ -477,8 +477,8 @@
             </a:outerShdw>
           </a:effectLst>
         </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
+      </effectStyleLst>
+      <bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -515,12 +515,12 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
+      </bgFillStyleLst>
+    </fmtScheme>
+  </themeElements>
+  <objectDefaults/>
+  <extraClrSchemeLst/>
+</theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
test: update snapshot test data
</commit_message>
<xml_diff>
--- a/cmd/ayd/testdata/log.xlsx
+++ b/cmd/ayd/testdata/log.xlsx
@@ -116,14 +116,13 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill/>
   </fills>
   <borders count="9">
     <border>
@@ -134,76 +133,44 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color rgb="FF89C923"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+    </border>
+    <border>
       <bottom style="thick">
         <color rgb="FF89C923"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+    </border>
+    <border>
       <bottom style="thin">
         <color rgb="FFFF2D00"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+    </border>
+    <border>
       <bottom style="thick">
         <color rgb="FFFF2D00"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+    </border>
+    <border>
       <bottom style="thin">
         <color rgb="FFC0C0C0"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+    </border>
+    <border>
       <bottom style="thick">
         <color rgb="FFC0C0C0"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+    </border>
+    <border>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+    </border>
+    <border>
       <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -214,7 +181,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="false">
       <alignment/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="false">
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="false">
       <alignment/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="false">
@@ -229,7 +196,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true" applyAlignment="false">
       <alignment/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="false">
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="false">
       <alignment/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="false">
@@ -241,19 +208,19 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="false">
       <alignment/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="false">
-      <alignment/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="false">
-      <alignment/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="false">
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="false">
+      <alignment/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="false">
+      <alignment/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="false">
       <alignment/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true" applyAlignment="false">
       <alignment/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="false">
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="false">
       <alignment/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="false">
@@ -268,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true" applyAlignment="false">
       <alignment/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="false">
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="false">
       <alignment/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="false">
@@ -280,7 +247,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="false">
       <alignment/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="false">
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="false">
       <alignment/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
test(logconv): Update Excel file for snapshot test
</commit_message>
<xml_diff>
--- a/cmd/ayd/testdata/log.xlsx
+++ b/cmd/ayd/testdata/log.xlsx
@@ -110,10 +110,10 @@
   </numFmts>
   <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">

</xml_diff>